<commit_message>
Tianyu Qi diary 03/17/2020
</commit_message>
<xml_diff>
--- a/diaries/diary-tianyu-qi.xlsx
+++ b/diaries/diary-tianyu-qi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\2-20_winter\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAF6742-DC2E-438F-9680-4708F6AED9BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A309AA32-D7B8-4D8F-B092-97A86BBD60FB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="193">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -602,6 +602,59 @@
   </si>
   <si>
     <t>You always need more patience. The development team looks much warmer on their own issues page than on Github. Why?</t>
+  </si>
+  <si>
+    <t>Last three KEPs. Advanced important topics to work on. Attitude adjustment. Some enduring principles. And a wrap-up for the quarter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Three KEPs. 
+2) Some other ways to see the codebase: history, visualization and refactoring.
+3) Nobody enjoys reading code, but attitudes make it fruitful or awful.
+4) Some enduring principles we should always follow. </t>
+  </si>
+  <si>
+    <t>Keep learning is a perfect las KEP for this class. There is so much we need to learn. And although the learning process is hard, it's always great to step out of our comfort zone. 
+It is interesting to see the code from a history way and also visualize the change.
+Reading code is never easy. But we've gone through a long way. And it's worth it.</t>
+  </si>
+  <si>
+    <t>Wonderful! Thanks Andre! Thanks Kaj! Thanks teammates! Thanks classmates!</t>
+  </si>
+  <si>
+    <t>3/13/2020
+3/15/2020</t>
+  </si>
+  <si>
+    <t>Solve the issue as much as I can.</t>
+  </si>
+  <si>
+    <t>Traced the code all the way down to what caused the problem and why it was there. Went as deep as I could. But it resulted in a generated file, which I cannot edit.</t>
+  </si>
+  <si>
+    <t>I really want to solve the issue.It looks interesting,  seems as a low-hang-fruit but takes a lot of time. It helped me so much in learning the parsing process of the Cassandra project. I never feel so confident when it comes to what I know about Cassandra.Unfortunately, I cannot solve it now. But I can actively communicate, and I will share the good news if there is any.</t>
+  </si>
+  <si>
+    <t>Happy and confident :D</t>
+  </si>
+  <si>
+    <t>8:00pm - 2:00am (3/17)</t>
+  </si>
+  <si>
+    <t>Finish a test case and the reports.</t>
+  </si>
+  <si>
+    <t>Wrote a new test case using Mockico, the tool I just learned from Jim's class. It feels so cool.
+Finished ALL the reports for this quarter!</t>
+  </si>
+  <si>
+    <t>It feels so good that classes are connected and knowledge is connected. This quarter was hard. But looking at ALL the reports we write for the classes, I feel that I did learn something.</t>
+  </si>
+  <si>
+    <t>Sleepy...Spring break begins!</t>
+  </si>
+  <si>
+    <t>1:00 - 9:00pm
+1:00 - 10:00pm</t>
   </si>
 </sst>
 </file>
@@ -782,7 +835,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -859,6 +912,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1178,24 +1240,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="90" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="29.5546875" customWidth="1"/>
-    <col min="5" max="5" width="46.88671875" customWidth="1"/>
-    <col min="6" max="6" width="48.33203125" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="20" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="5" max="5" width="46.85546875" customWidth="1"/>
+    <col min="6" max="6" width="48.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -1206,7 +1268,7 @@
       <c r="F1" s="26"/>
       <c r="G1" s="26"/>
     </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1215,7 +1277,7 @@
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
     </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="17"/>
       <c r="C3" s="1"/>
@@ -1224,7 +1286,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1237,7 +1299,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1250,7 +1312,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1263,7 +1325,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="17"/>
       <c r="C7" s="1"/>
@@ -1272,7 +1334,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="7"/>
       <c r="C8" s="4"/>
@@ -1281,7 +1343,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1304,7 +1366,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>14</v>
       </c>
@@ -1327,7 +1389,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="11" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="11" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>19</v>
       </c>
@@ -1350,7 +1412,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="11" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="11" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>27</v>
       </c>
@@ -1373,7 +1435,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="11" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>32</v>
       </c>
@@ -1396,7 +1458,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="11" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="11" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>39</v>
       </c>
@@ -1419,7 +1481,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>44</v>
       </c>
@@ -1442,7 +1504,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="11" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="11" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>49</v>
       </c>
@@ -1465,7 +1527,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="14" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="14" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>57</v>
       </c>
@@ -1488,7 +1550,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="14" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="14" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>64</v>
       </c>
@@ -1511,7 +1573,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="21" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="21" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>68</v>
       </c>
@@ -1534,7 +1596,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="21" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>72</v>
       </c>
@@ -1557,7 +1619,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>77</v>
       </c>
@@ -1580,7 +1642,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="11" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>77</v>
       </c>
@@ -1603,7 +1665,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="21" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="21" customFormat="1" ht="126" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>98</v>
       </c>
@@ -1626,7 +1688,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="11" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" s="11" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>100</v>
       </c>
@@ -1649,7 +1711,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="11" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" s="11" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>105</v>
       </c>
@@ -1672,7 +1734,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="11" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" s="11" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>112</v>
       </c>
@@ -1695,7 +1757,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="11" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" s="11" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>115</v>
       </c>
@@ -1718,7 +1780,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="11" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>123</v>
       </c>
@@ -1741,7 +1803,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="11" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" s="11" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>128</v>
       </c>
@@ -1764,7 +1826,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="11" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" s="11" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>131</v>
       </c>
@@ -1787,7 +1849,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="11" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" s="11" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>132</v>
       </c>
@@ -1810,7 +1872,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="11" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" s="11" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>133</v>
       </c>
@@ -1833,7 +1895,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="11" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" s="11" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>137</v>
       </c>
@@ -1856,7 +1918,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="24" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="24" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A34" s="22">
         <v>43891</v>
       </c>
@@ -1879,7 +1941,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="24" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="22">
         <v>43893</v>
       </c>
@@ -1902,7 +1964,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="24" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" s="24" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
         <v>43895</v>
       </c>
@@ -1925,7 +1987,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="24" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" s="24" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>173</v>
       </c>
@@ -1948,7 +2010,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="11" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" s="11" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="22">
         <v>43901</v>
       </c>
@@ -1971,58 +2033,94 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="25">
+    <row r="39" spans="1:7" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+      <c r="A39" s="22">
         <v>43902</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="8"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="25"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="8"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="8"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D39" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="24" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A41" s="22">
+        <v>43906</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="G41" s="23" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="29" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="25"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="28"/>
+    </row>
+    <row r="43" spans="1:7" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="22"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="23"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -2031,7 +2129,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -2040,7 +2138,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -2049,7 +2147,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -2058,7 +2156,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -2067,7 +2165,7 @@
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -2076,7 +2174,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -2085,7 +2183,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -2094,7 +2192,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -2103,7 +2201,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -2112,7 +2210,7 @@
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -2121,7 +2219,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -2130,7 +2228,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -2139,7 +2237,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -2148,7 +2246,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -2157,7 +2255,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -2166,7 +2264,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -2175,7 +2273,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -2184,7 +2282,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -2193,7 +2291,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -2202,7 +2300,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -2211,7 +2309,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -2220,7 +2318,7 @@
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -2229,7 +2327,7 @@
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -2238,7 +2336,7 @@
       <c r="F67" s="7"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -2247,7 +2345,7 @@
       <c r="F68" s="7"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -2256,7 +2354,7 @@
       <c r="F69" s="7"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -2265,7 +2363,7 @@
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -2274,7 +2372,7 @@
       <c r="F71" s="7"/>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -2283,7 +2381,7 @@
       <c r="F72" s="7"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -2292,7 +2390,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -2301,7 +2399,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -2310,7 +2408,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -2319,7 +2417,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -2328,7 +2426,7 @@
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -2337,7 +2435,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -2346,7 +2444,7 @@
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -2355,7 +2453,7 @@
       <c r="F80" s="7"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -2364,7 +2462,7 @@
       <c r="F81" s="7"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -2373,7 +2471,7 @@
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -2382,7 +2480,7 @@
       <c r="F83" s="7"/>
       <c r="G83" s="8"/>
     </row>
-    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -2391,7 +2489,7 @@
       <c r="F84" s="7"/>
       <c r="G84" s="8"/>
     </row>
-    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -2400,7 +2498,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -2409,7 +2507,7 @@
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
     </row>
-    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -2418,7 +2516,7 @@
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
     </row>
-    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -2427,7 +2525,7 @@
       <c r="F88" s="7"/>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -2436,7 +2534,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="8"/>
     </row>
-    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -2445,7 +2543,7 @@
       <c r="F90" s="7"/>
       <c r="G90" s="8"/>
     </row>
-    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -2454,7 +2552,7 @@
       <c r="F91" s="7"/>
       <c r="G91" s="8"/>
     </row>
-    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -2463,7 +2561,7 @@
       <c r="F92" s="7"/>
       <c r="G92" s="8"/>
     </row>
-    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -2472,7 +2570,7 @@
       <c r="F93" s="7"/>
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -2481,7 +2579,7 @@
       <c r="F94" s="7"/>
       <c r="G94" s="8"/>
     </row>
-    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -2490,7 +2588,7 @@
       <c r="F95" s="7"/>
       <c r="G95" s="8"/>
     </row>
-    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -2499,7 +2597,7 @@
       <c r="F96" s="7"/>
       <c r="G96" s="8"/>
     </row>
-    <row r="97" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -2508,7 +2606,7 @@
       <c r="F97" s="7"/>
       <c r="G97" s="8"/>
     </row>
-    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -2517,7 +2615,7 @@
       <c r="F98" s="7"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -2526,7 +2624,7 @@
       <c r="F99" s="7"/>
       <c r="G99" s="8"/>
     </row>
-    <row r="100" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -2535,7 +2633,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="8"/>
     </row>
-    <row r="101" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -2544,7 +2642,7 @@
       <c r="F101" s="7"/>
       <c r="G101" s="8"/>
     </row>
-    <row r="102" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -2553,7 +2651,7 @@
       <c r="F102" s="7"/>
       <c r="G102" s="8"/>
     </row>
-    <row r="103" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -2562,7 +2660,7 @@
       <c r="F103" s="7"/>
       <c r="G103" s="8"/>
     </row>
-    <row r="104" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -2571,7 +2669,7 @@
       <c r="F104" s="7"/>
       <c r="G104" s="8"/>
     </row>
-    <row r="105" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -2580,7 +2678,7 @@
       <c r="F105" s="7"/>
       <c r="G105" s="8"/>
     </row>
-    <row r="106" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -2589,7 +2687,7 @@
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
     </row>
-    <row r="107" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -2598,7 +2696,7 @@
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
     </row>
-    <row r="108" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -2607,7 +2705,7 @@
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
     </row>
-    <row r="109" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -2616,7 +2714,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
     </row>
-    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -2625,7 +2723,7 @@
       <c r="F110" s="7"/>
       <c r="G110" s="8"/>
     </row>
-    <row r="111" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -2634,7 +2732,7 @@
       <c r="F111" s="7"/>
       <c r="G111" s="8"/>
     </row>
-    <row r="112" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -2643,7 +2741,7 @@
       <c r="F112" s="7"/>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -2652,7 +2750,7 @@
       <c r="F113" s="7"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -2661,7 +2759,7 @@
       <c r="F114" s="7"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -2670,7 +2768,7 @@
       <c r="F115" s="7"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -2679,7 +2777,7 @@
       <c r="F116" s="7"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -2688,7 +2786,7 @@
       <c r="F117" s="7"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -2697,7 +2795,7 @@
       <c r="F118" s="7"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -2706,7 +2804,7 @@
       <c r="F119" s="7"/>
       <c r="G119" s="8"/>
     </row>
-    <row r="120" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -2715,7 +2813,7 @@
       <c r="F120" s="7"/>
       <c r="G120" s="8"/>
     </row>
-    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -2724,7 +2822,7 @@
       <c r="F121" s="7"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -2733,7 +2831,7 @@
       <c r="F122" s="7"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -2742,7 +2840,7 @@
       <c r="F123" s="7"/>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -2750,6 +2848,15 @@
       <c r="E124" s="7"/>
       <c r="F124" s="7"/>
       <c r="G124" s="8"/>
+    </row>
+    <row r="125" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A125" s="7"/>
+      <c r="B125" s="7"/>
+      <c r="C125" s="7"/>
+      <c r="D125" s="7"/>
+      <c r="E125" s="7"/>
+      <c r="F125" s="7"/>
+      <c r="G125" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>